<commit_message>
Some final documentation updates
End of semester submission
</commit_message>
<xml_diff>
--- a/Documentation/Time Logging.xlsx
+++ b/Documentation/Time Logging.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Milestone 4 Presentation</t>
   </si>
+  <si>
+    <t>Milestone 5 due (Design)</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -84,13 +87,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -113,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -130,6 +144,18 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -414,7 +440,7 @@
       </c>
       <c r="H4" s="8">
         <f>SUM(B:B)</f>
-        <v>34</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -431,7 +457,7 @@
       </c>
       <c r="H5" s="8">
         <f>SUM(C:C)</f>
-        <v>14</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -477,7 +503,7 @@
       </c>
       <c r="H7" s="8">
         <f>SUM(E:E)</f>
-        <v>28</v>
+        <v>111.5</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -491,6 +517,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="6"/>
+      <c r="H8" s="10">
+        <f>SUM(H4,H5,H6,H7)</f>
+        <v>306.5</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1">
@@ -771,7 +801,9 @@
       <c r="B31" s="3">
         <v>5.0</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="3">
+        <v>4.0</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3">
         <v>3.0</v>
@@ -785,7 +817,9 @@
       <c r="B32" s="3">
         <v>2.0</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="3">
+        <v>2.0</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3">
         <v>2.0</v>
@@ -799,7 +833,9 @@
       <c r="B33" s="3">
         <v>3.0</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3">
         <v>3.0</v>
@@ -813,7 +849,9 @@
       <c r="B34" s="3">
         <v>8.0</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="3">
+        <v>6.0</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3">
         <v>5.0</v>
@@ -826,7 +864,9 @@
       <c r="A35" s="1">
         <v>44010.0</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
@@ -836,10 +876,16 @@
       <c r="A36" s="1">
         <v>44011.0</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
+      <c r="E36" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F36" s="4" t="s">
         <v>10</v>
       </c>
@@ -858,20 +904,32 @@
       <c r="A38" s="1">
         <v>44013.0</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3">
+        <v>2.0</v>
+      </c>
       <c r="F38" s="6"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1">
         <v>44014.0</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="3">
+        <v>4.0</v>
+      </c>
       <c r="F39" s="6"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -888,7 +946,9 @@
       <c r="A41" s="1">
         <v>44016.0</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
@@ -898,7 +958,9 @@
       <c r="A42" s="1">
         <v>44017.0</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -928,7 +990,9 @@
       <c r="A45" s="1">
         <v>44020.0</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -948,7 +1012,9 @@
       <c r="A47" s="1">
         <v>44022.0</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -958,7 +1024,9 @@
       <c r="A48" s="1">
         <v>44023.0</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -978,7 +1046,9 @@
       <c r="A50" s="1">
         <v>44025.0</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -988,7 +1058,9 @@
       <c r="A51" s="1">
         <v>44026.0</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1018,7 +1090,9 @@
       <c r="A54" s="1">
         <v>44029.0</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1028,7 +1102,9 @@
       <c r="A55" s="1">
         <v>44030.0</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1048,50 +1124,72 @@
       <c r="A57" s="1">
         <v>44032.0</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="E57" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F57" s="6"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1">
         <v>44033.0</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="E58" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1">
         <v>44034.0</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="3">
+        <v>2.0</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="E59" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F59" s="6"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1">
         <v>44035.0</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="3">
+        <v>4.0</v>
+      </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+      <c r="E60" s="3">
+        <v>1.0</v>
+      </c>
       <c r="F60" s="6"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1">
         <v>44036.0</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="E61" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F61" s="4" t="s">
         <v>11</v>
       </c>
@@ -1100,30 +1198,48 @@
       <c r="A62" s="1">
         <v>44037.0</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="B62" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C62" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="E62" s="3">
+        <v>4.0</v>
+      </c>
       <c r="F62" s="6"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1">
         <v>44038.0</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C63" s="3">
+        <v>2.0</v>
+      </c>
       <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+      <c r="E63" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F63" s="6"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1">
         <v>44039.0</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C64" s="3">
+        <v>4.0</v>
+      </c>
       <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="E64" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F64" s="4" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1251,9 @@
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="E65" s="3">
+        <v>2.0</v>
+      </c>
       <c r="F65" s="6"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
@@ -1145,7 +1263,9 @@
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="E66" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F66" s="4"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -1155,7 +1275,9 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="E67" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F67" s="6"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -1165,7 +1287,9 @@
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="E68" s="3">
+        <v>5.0</v>
+      </c>
       <c r="F68" s="6"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
@@ -1173,7 +1297,9 @@
         <v>44044.0</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="C69" s="3">
+        <v>5.0</v>
+      </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="6"/>
@@ -1182,10 +1308,14 @@
       <c r="A70" s="1">
         <v>44045.0</v>
       </c>
-      <c r="B70" s="2"/>
+      <c r="B70" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="E70" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F70" s="6"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -1195,7 +1325,9 @@
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="E71" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F71" s="6"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -1212,8 +1344,12 @@
       <c r="A73" s="1">
         <v>44048.0</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="B73" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C73" s="3">
+        <v>7.0</v>
+      </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="6"/>
@@ -1225,27 +1361,37 @@
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="E74" s="3">
+        <v>4.0</v>
+      </c>
       <c r="F74" s="6"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1">
         <v>44050.0</v>
       </c>
-      <c r="B75" s="2"/>
+      <c r="B75" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+      <c r="E75" s="3">
+        <v>3.5</v>
+      </c>
       <c r="F75" s="6"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1">
         <v>44051.0</v>
       </c>
-      <c r="B76" s="2"/>
+      <c r="B76" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
+      <c r="E76" s="3">
+        <v>6.0</v>
+      </c>
       <c r="F76" s="6"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
@@ -1255,37 +1401,55 @@
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
+      <c r="E77" s="3">
+        <v>5.5</v>
+      </c>
       <c r="F77" s="6"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="1">
         <v>44053.0</v>
       </c>
-      <c r="B78" s="2"/>
+      <c r="B78" s="3">
+        <v>4.0</v>
+      </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
+      <c r="E78" s="3">
+        <v>2.0</v>
+      </c>
       <c r="F78" s="6"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1">
         <v>44054.0</v>
       </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="B79" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C79" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="6"/>
+      <c r="E79" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1">
         <v>44055.0</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="C80" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="E80" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F80" s="6"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
@@ -1295,7 +1459,9 @@
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="E81" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F81" s="6"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -1305,7 +1471,9 @@
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+      <c r="E82" s="12">
+        <v>2.0</v>
+      </c>
       <c r="F82" s="6"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -1313,9 +1481,13 @@
         <v>44058.0</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="C83" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+      <c r="E83" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F83" s="6"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
@@ -1325,7 +1497,9 @@
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="E84" s="3">
+        <v>4.5</v>
+      </c>
       <c r="F84" s="6"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
@@ -1335,45 +1509,69 @@
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="E85" s="3">
+        <v>2.0</v>
+      </c>
       <c r="F85" s="6"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="1">
         <v>44061.0</v>
       </c>
-      <c r="B86" s="2"/>
+      <c r="B86" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
+      <c r="E86" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F86" s="6"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="1">
         <v>44062.0</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="B87" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3.0</v>
+      </c>
       <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="E87" s="3">
+        <v>0.0</v>
+      </c>
       <c r="F87" s="6"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1">
         <v>44063.0</v>
       </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="B88" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C88" s="3">
+        <v>5.0</v>
+      </c>
       <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+      <c r="E88" s="3">
+        <v>2.0</v>
+      </c>
       <c r="F88" s="6"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="1"/>
-      <c r="B89" s="2"/>
+      <c r="A89" s="13">
+        <v>44064.0</v>
+      </c>
+      <c r="B89" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+      <c r="E89" s="3">
+        <v>3.0</v>
+      </c>
       <c r="F89" s="6"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">

</xml_diff>